<commit_message>
Updated possible concentrations file to include the active learning concentrations
</commit_message>
<xml_diff>
--- a/Supplementary/possible_concentrations.xlsx
+++ b/Supplementary/possible_concentrations.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conar\Memplex_platform\Supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6283995E-AA1A-4AD9-A197-953F9A2F7A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25499E5-D272-4C17-A2B5-E406114CC773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{37340067-43D3-4DFB-AD64-18EE3332C85A}"/>
+    <workbookView xWindow="-72" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{37340067-43D3-4DFB-AD64-18EE3332C85A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="39">
   <si>
     <t>reagent</t>
   </si>
@@ -113,49 +113,49 @@
     <t>FFAR4</t>
   </si>
   <si>
-    <t>Liposome</t>
+    <t>Aux</t>
+  </si>
+  <si>
+    <t>B2AR</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>CD47</t>
+  </si>
+  <si>
+    <t>CaM</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Glut</t>
+  </si>
+  <si>
+    <t>InP</t>
+  </si>
+  <si>
+    <t>Mito</t>
+  </si>
+  <si>
+    <t>Mol</t>
+  </si>
+  <si>
+    <t>Neu</t>
+  </si>
+  <si>
+    <t>Vol</t>
+  </si>
+  <si>
+    <t>Liposome_name</t>
   </si>
   <si>
     <t>DOPC</t>
   </si>
   <si>
     <t>DMPC</t>
-  </si>
-  <si>
-    <t>Aux</t>
-  </si>
-  <si>
-    <t>B2AR</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>CD47</t>
-  </si>
-  <si>
-    <t>CaM</t>
-  </si>
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Glut</t>
-  </si>
-  <si>
-    <t>InP</t>
-  </si>
-  <si>
-    <t>Mito</t>
-  </si>
-  <si>
-    <t>Mol</t>
-  </si>
-  <si>
-    <t>Neu</t>
-  </si>
-  <si>
-    <t>Vol</t>
   </si>
 </sst>
 </file>
@@ -507,15 +507,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036AE11B-0F92-4472-B21E-57C4994B691E}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -537,29 +537,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -570,29 +570,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -603,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -614,7 +614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -625,7 +625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -636,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -647,18 +647,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -669,18 +669,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -691,51 +691,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
       <c r="C20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -746,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -757,18 +757,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -779,7 +779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -790,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -801,7 +801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -823,18 +823,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -845,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -853,134 +853,189 @@
         <v>4</v>
       </c>
       <c r="C31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37">
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B42" t="s">
         <v>6</v>
       </c>
-      <c r="C36">
+      <c r="C42">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>6</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B43" t="s">
         <v>6</v>
       </c>
-      <c r="C37">
+      <c r="C43">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44">
         <v>1.25</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>7</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C38">
+      <c r="C45">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>7</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="C39">
+      <c r="C46">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>7</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B47" t="s">
         <v>7</v>
       </c>
-      <c r="C40">
+      <c r="C47">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C42" xr:uid="{036AE11B-0F92-4472-B21E-57C4994B691E}">
+  <autoFilter ref="A1:C46" xr:uid="{036AE11B-0F92-4472-B21E-57C4994B691E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C28">
-      <sortCondition ref="B1:B42"/>
+      <sortCondition ref="B1:B46"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>